<commit_message>
big changes (close to final)
added variable fast-forward speed (change via front-end settings menu)

added a confirmation sequence (just for food trial sets)

added a start menu before each video (requires input - mouse or keyboard - to start a video playback)

changed some of the colours of the feedback banners to more accurately match the experiment's

improved fidelity check -  now it will reflect if the coder noticed a wrong food in the bowl

added some comments for clarity

removed redundant variables that were a remnant from back when the program was completely different
</commit_message>
<xml_diff>
--- a/testsheet.xlsx
+++ b/testsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kelvin Zhou\Box Sync\DUKE\Psych\Huettel Lab\veggie-table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AF6E811-1164-46DA-B3EA-4FDD8C1E6B59}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5DE3876-F24A-41B0-9D03-04771BAFF785}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="465" windowWidth="31995" windowHeight="24000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -452,7 +452,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>

</xml_diff>